<commit_message>
LS_Trafo is added v1
</commit_message>
<xml_diff>
--- a/Sankar Action Items.xlsx
+++ b/Sankar Action Items.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26626"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sankar S\Desktop\Sankar Action\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB27DBB-4C25-471D-8CF6-09A3F2F64D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10305"/>
   </bookViews>
   <sheets>
     <sheet name="Action Item" sheetId="1" r:id="rId1"/>
@@ -25,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="10">
   <si>
     <t>Capacitor Design</t>
   </si>
@@ -55,21 +49,12 @@
   </si>
   <si>
     <t>4th July 2023</t>
-  </si>
-  <si>
-    <t>hi added</t>
-  </si>
-  <si>
-    <t>hi content added</t>
-  </si>
-  <si>
-    <t>added</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,28 +403,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.1796875" customWidth="1"/>
-    <col min="2" max="2" width="13.54296875" customWidth="1"/>
-    <col min="3" max="3" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" width="55.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.85546875" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -450,7 +436,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -459,7 +445,7 @@
       </c>
       <c r="C2" s="4"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
@@ -468,7 +454,7 @@
       </c>
       <c r="C3" s="4"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
@@ -477,7 +463,7 @@
       </c>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -486,8 +472,8 @@
       </c>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
@@ -495,7 +481,7 @@
       </c>
       <c r="C6" s="4"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>8</v>
       </c>
@@ -504,21 +490,13 @@
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>12</v>
-      </c>
-    </row>
+    <row r="8" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="14.45" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+    </row>
+    <row r="11" spans="1:3" ht="14.45" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="C1:C7"/>

</xml_diff>